<commit_message>
Content matrix à Hugo
</commit_message>
<xml_diff>
--- a/Document/ContentMatrix.xlsx
+++ b/Document/ContentMatrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prog\INFO s5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1372883\Documents\Projet de bd\Servider\Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="840" firstSheet="2" activeTab="3"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="840" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Légende" sheetId="1" r:id="rId1"/>
@@ -1374,9 +1374,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1384,6 +1381,9 @@
     <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="31" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="11" xfId="31" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="32">
@@ -1805,11 +1805,11 @@
   <sheetData>
     <row r="1" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="2" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="109" t="s">
+      <c r="B2" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="109"/>
-      <c r="D2" s="109"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="102" t="s">
@@ -2014,8 +2014,8 @@
   <dimension ref="A1:R856"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="G30"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2117,10 +2117,10 @@
       <c r="I2" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="113" t="s">
+      <c r="J2" s="112" t="s">
         <v>54</v>
       </c>
-      <c r="K2" s="113" t="s">
+      <c r="K2" s="112" t="s">
         <v>55</v>
       </c>
       <c r="L2" s="60"/>
@@ -2293,10 +2293,10 @@
       <c r="I6" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="J6" s="112" t="s">
+      <c r="J6" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="K6" s="111" t="s">
+      <c r="K6" s="110" t="s">
         <v>76</v>
       </c>
       <c r="L6" s="28"/>
@@ -2547,10 +2547,10 @@
       <c r="I12" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="111" t="s">
+      <c r="J12" s="110" t="s">
         <v>101</v>
       </c>
-      <c r="K12" s="110" t="s">
+      <c r="K12" s="109" t="s">
         <v>102</v>
       </c>
       <c r="L12" s="28"/>
@@ -3094,7 +3094,7 @@
         <v>44</v>
       </c>
       <c r="J25" s="40" t="str">
-        <f t="shared" ref="J25:K25" si="0">J9</f>
+        <f t="shared" ref="J25" si="0">J9</f>
         <v>[Password]</v>
       </c>
       <c r="K25" s="40" t="str">
@@ -3325,7 +3325,9 @@
     </row>
     <row r="31" spans="1:18" s="18" customFormat="1" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="36"/>
-      <c r="B31" s="27"/>
+      <c r="B31" s="27">
+        <v>4</v>
+      </c>
       <c r="C31" s="43"/>
       <c r="D31" s="34"/>
       <c r="E31" s="39"/>
@@ -19781,12 +19783,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -19839,15 +19838,24 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -19868,15 +19876,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{30E84F96-43E5-4C3A-8E0E-76AD01F7D6A1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{56277F14-5102-450B-9F74-CC1199F0A7EB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>